<commit_message>
Updated recovery dates from Quick Look Cruise Report
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP02PMUI_00006.xlsx
+++ b/deployment/Omaha_Cal_Info_CP02PMUI_00006.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13035" yWindow="6300" windowWidth="21480" windowHeight="11235" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="13035" yWindow="6300" windowWidth="21480" windowHeight="11235" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,7 +1034,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="G2" s="2">
-        <v>42510</v>
+        <v>42511</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>51</v>
@@ -1077,7 +1077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>

</xml_diff>